<commit_message>
Reviewed and validated bi-weekly gw data
* added welltop to ground measurements from Aug 2020
* added well depth measurements from Aug 2020
* split welltop to ground measurements from well depth measurements into separate files
* reviewed Laura Murtagh's master data and notes, validated
* added well meter offset raw data and averages
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/Wells_with_Missing_Data.xlsx
+++ b/data/field_observations/groundwater/Wells_with_Missing_Data.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/field-based/groundwater/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AEF169-2A09-AF40-B6B1-426F91CD92F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FB5923-0BE3-A34B-9F39-C3E651E072FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38260" yWindow="580" windowWidth="10000" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>No top2gnd</t>
   </si>
@@ -28,12 +39,6 @@
     <t>KHF-XD4S</t>
   </si>
   <si>
-    <t>EFR-XB2S</t>
-  </si>
-  <si>
-    <t>EFR-XB3S</t>
-  </si>
-  <si>
     <t>KER-XE3S</t>
   </si>
   <si>
@@ -64,9 +69,6 @@
     <t>KET-1</t>
   </si>
   <si>
-    <t>KWR-XD1N</t>
-  </si>
-  <si>
     <t>KHF-XE7S</t>
   </si>
   <si>
@@ -85,12 +87,6 @@
     <t>EWR-1</t>
   </si>
   <si>
-    <t>EFR-XB1S</t>
-  </si>
-  <si>
-    <t>EEF-1</t>
-  </si>
-  <si>
     <t>KHR-XD2N</t>
   </si>
   <si>
@@ -110,24 +106,6 @@
   </si>
   <si>
     <t>KWR-1</t>
-  </si>
-  <si>
-    <t>EHR-XB1N</t>
-  </si>
-  <si>
-    <t>EFR-XB2N</t>
-  </si>
-  <si>
-    <t>EFR-XB3N</t>
-  </si>
-  <si>
-    <t>EWR-XB4N</t>
-  </si>
-  <si>
-    <t>KRH-XD1S</t>
-  </si>
-  <si>
-    <t>EFF-XB7S</t>
   </si>
 </sst>
 </file>
@@ -484,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -501,7 +479,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -509,7 +487,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -517,7 +495,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -525,188 +503,136 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>33</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="B18" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="B19" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B29" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="B25" s="1"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="B30" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated filenames and column names
</commit_message>
<xml_diff>
--- a/data/field_observations/groundwater/Wells_with_Missing_Data.xlsx
+++ b/data/field_observations/groundwater/Wells_with_Missing_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jnat/Documents/GitHub/sagehen_meadows/data/field_observations/groundwater/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FB5923-0BE3-A34B-9F39-C3E651E072FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A49024-9351-0940-B819-55B66D3FDCF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38260" yWindow="580" windowWidth="10000" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7280" yWindow="1940" windowWidth="15060" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
   <si>
     <t>No top2gnd</t>
   </si>
@@ -106,16 +106,74 @@
   </si>
   <si>
     <t>KWR-1</t>
+  </si>
+  <si>
+    <t>No LogHole to WellTop</t>
+  </si>
+  <si>
+    <t>KER-1</t>
+  </si>
+  <si>
+    <t>KHT-XE5S</t>
+  </si>
+  <si>
+    <t>KWT-1</t>
+  </si>
+  <si>
+    <t>EHT-XA5S</t>
+  </si>
+  <si>
+    <t>EEF-1</t>
+  </si>
+  <si>
+    <t>EET-1</t>
+  </si>
+  <si>
+    <t>KWF-1</t>
+  </si>
+  <si>
+    <t>KEFR-XE1A</t>
+  </si>
+  <si>
+    <t>A3S</t>
+  </si>
+  <si>
+    <t>EWT-1</t>
+  </si>
+  <si>
+    <t>EWF-XA2S</t>
+  </si>
+  <si>
+    <t>KHT-XE4S</t>
+  </si>
+  <si>
+    <t>KHF-1</t>
+  </si>
+  <si>
+    <t>LHR-1</t>
+  </si>
+  <si>
+    <t>E5S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -145,9 +203,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,179 +522,333 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="1"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C26" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B30" s="1"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F40" s="3"/>
+    </row>
+    <row r="41" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F46" s="3"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F7:F46">
+    <sortCondition ref="F7:F46"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>